<commit_message>
Bug fix in init
Fixed bug when selecting container type that's allowed
</commit_message>
<xml_diff>
--- a/readLite.xlsx
+++ b/readLite.xlsx
@@ -52,9 +52,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -359,9 +358,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A19"/>
+  <dimension ref="A1:A31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -371,93 +372,153 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>54.279999829530702</v>
+      <c r="A2">
+        <v>21.31</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>174.51999974250799</v>
+      <c r="A3">
+        <v>89.59</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>983.400001093745</v>
+      <c r="A4">
+        <v>9.35</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>3546.5599960088698</v>
+      <c r="A5">
+        <v>68.040000000000006</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>7.7000001072883597</v>
+      <c r="A6">
+        <v>82.91</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>5.93999996781349</v>
+      <c r="A7">
+        <v>1767.45</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>1.0099999904632599</v>
+      <c r="A8">
+        <v>5.38</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>72.879999369382901</v>
+      <c r="A9">
+        <v>660.56</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>44.199999183416402</v>
+      <c r="A10">
+        <v>20.059999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>14.0499998307228</v>
+      <c r="A11">
+        <v>0.27</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>6.1100000292062804</v>
+      <c r="A12">
+        <v>3.42</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>336.31000149250002</v>
+      <c r="A13">
+        <v>0.17</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>91.319999486208005</v>
+      <c r="A14">
+        <v>7.75</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>249.15000149607701</v>
+      <c r="A15">
+        <v>4.07</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>1.66999995708466</v>
+      <c r="A16">
+        <v>42.32</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>640.05000294446995</v>
+      <c r="A17">
+        <v>97.05</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>4.4099999964237204</v>
+      <c r="A18">
+        <v>70.17</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>1.54999995231628</v>
+      <c r="A19">
+        <v>2.38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>5.51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>272.08999999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>11.37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>66.61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>17.03</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>104.52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>213.02</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27.75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>3.46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>217.04</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>19.239999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Compatible with 3.5 and 3.7
</commit_message>
<xml_diff>
--- a/readLite.xlsx
+++ b/readLite.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$A$1</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
@@ -358,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -373,20 +376,26 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>82</v>
+        <v>29.73</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>159</v>
+        <v>11.12</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>69.91</v>
+        <v>41.19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>32.020000000000003</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>